<commit_message>
more verbs -> identifiers
</commit_message>
<xml_diff>
--- a/Adventure.xlsx
+++ b/Adventure.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Adventure-wherigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874A9B19-A8C5-4143-97B9-F6372E4C0359}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39530E3-E482-4DAF-9385-C1AAD07BEA0E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="10790" xr2:uid="{DA9CDC86-6B9C-4A3C-A222-7CC08085C3FF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="10790" activeTab="4" xr2:uid="{DA9CDC86-6B9C-4A3C-A222-7CC08085C3FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
     <sheet name="Objects" sheetId="2" r:id="rId2"/>
     <sheet name="Characters" sheetId="3" r:id="rId3"/>
     <sheet name="Magic words" sheetId="4" r:id="rId4"/>
+    <sheet name="verbs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="425">
   <si>
     <t>Long description</t>
   </si>
@@ -1081,6 +1082,228 @@
   </si>
   <si>
     <t>You appear to be lost in a dark and gloomy forest.</t>
+  </si>
+  <si>
+    <t>blast</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>brief</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>climb</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>cross</t>
+  </si>
+  <si>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>dig</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>drop</t>
+  </si>
+  <si>
+    <t>free, dr</t>
+  </si>
+  <si>
+    <t>eat</t>
+  </si>
+  <si>
+    <t>enter</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>exit</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>extinguish</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>feed</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>walk, run</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>g, take</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>hoot</t>
+  </si>
+  <si>
+    <t>info</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I </t>
+  </si>
+  <si>
+    <t>jump</t>
+  </si>
+  <si>
+    <t>kill</t>
+  </si>
+  <si>
+    <t>lift</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>listen</t>
+  </si>
+  <si>
+    <t>look</t>
+  </si>
+  <si>
+    <t>l, examine, x</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>unlock</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>pour</t>
+  </si>
+  <si>
+    <t>quit</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>reflect</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>rest</t>
+  </si>
+  <si>
+    <t>restore</t>
+  </si>
+  <si>
+    <t>retreat</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>ride</t>
+  </si>
+  <si>
+    <t>rub</t>
+  </si>
+  <si>
+    <t>polish</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>say</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>scry</t>
+  </si>
+  <si>
+    <t>tame</t>
+  </si>
+  <si>
+    <t>placate</t>
+  </si>
+  <si>
+    <t>terse</t>
+  </si>
+  <si>
+    <t>throw</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>translate</t>
+  </si>
+  <si>
+    <t>verbose</t>
+  </si>
+  <si>
+    <t>wash</t>
+  </si>
+  <si>
+    <t>wave</t>
+  </si>
+  <si>
+    <t>swing</t>
+  </si>
+  <si>
+    <t>wear</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738AE1BC-ED79-46FF-9BB3-5FA0937E704C}">
   <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D132" sqref="D132"/>
     </sheetView>
@@ -6062,4 +6285,521 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82045E9-E42F-446C-9E79-EEE8F9C54219}">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B3">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B5">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>356</v>
+      </c>
+      <c r="B6">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>358</v>
+      </c>
+      <c r="B8">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>359</v>
+      </c>
+      <c r="B9">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>360</v>
+      </c>
+      <c r="B10">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11">
+        <v>535</v>
+      </c>
+      <c r="C11" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>363</v>
+      </c>
+      <c r="B12">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B13">
+        <v>526</v>
+      </c>
+      <c r="C13" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>366</v>
+      </c>
+      <c r="B14">
+        <v>527</v>
+      </c>
+      <c r="C14" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>368</v>
+      </c>
+      <c r="B15">
+        <v>546</v>
+      </c>
+      <c r="C15" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>370</v>
+      </c>
+      <c r="B16">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B17">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>372</v>
+      </c>
+      <c r="B18">
+        <v>528</v>
+      </c>
+      <c r="C18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>374</v>
+      </c>
+      <c r="B19">
+        <v>534</v>
+      </c>
+      <c r="C19" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>376</v>
+      </c>
+      <c r="B20">
+        <v>580</v>
+      </c>
+      <c r="C20" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>378</v>
+      </c>
+      <c r="B21">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>379</v>
+      </c>
+      <c r="B22">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>380</v>
+      </c>
+      <c r="B23">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>381</v>
+      </c>
+      <c r="B24">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>382</v>
+      </c>
+      <c r="B25">
+        <v>594</v>
+      </c>
+      <c r="C25" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>384</v>
+      </c>
+      <c r="B26">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>385</v>
+      </c>
+      <c r="B27">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>386</v>
+      </c>
+      <c r="B28">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>387</v>
+      </c>
+      <c r="B29">
+        <v>545</v>
+      </c>
+      <c r="C29" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>389</v>
+      </c>
+      <c r="B30">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>390</v>
+      </c>
+      <c r="B31">
+        <v>571</v>
+      </c>
+      <c r="C31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>392</v>
+      </c>
+      <c r="B32">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>393</v>
+      </c>
+      <c r="B33">
+        <v>536</v>
+      </c>
+      <c r="C33" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>395</v>
+      </c>
+      <c r="B34">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>396</v>
+      </c>
+      <c r="B35">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>397</v>
+      </c>
+      <c r="B36">
+        <v>572</v>
+      </c>
+      <c r="C36" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>399</v>
+      </c>
+      <c r="B37">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>400</v>
+      </c>
+      <c r="B38">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>401</v>
+      </c>
+      <c r="B39">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>402</v>
+      </c>
+      <c r="B40">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>403</v>
+      </c>
+      <c r="B41">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>404</v>
+      </c>
+      <c r="B42">
+        <v>530</v>
+      </c>
+      <c r="C42" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>406</v>
+      </c>
+      <c r="B43">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>407</v>
+      </c>
+      <c r="B44">
+        <v>556</v>
+      </c>
+      <c r="C44" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>409</v>
+      </c>
+      <c r="B45">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>410</v>
+      </c>
+      <c r="B46">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>411</v>
+      </c>
+      <c r="B47">
+        <v>595</v>
+      </c>
+      <c r="C47" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>413</v>
+      </c>
+      <c r="B48">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>414</v>
+      </c>
+      <c r="B49">
+        <v>548</v>
+      </c>
+      <c r="C49" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>416</v>
+      </c>
+      <c r="B50">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>417</v>
+      </c>
+      <c r="B51">
+        <v>557</v>
+      </c>
+      <c r="C51" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>419</v>
+      </c>
+      <c r="B52">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>420</v>
+      </c>
+      <c r="B53">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>421</v>
+      </c>
+      <c r="B54">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>422</v>
+      </c>
+      <c r="B55">
+        <v>547</v>
+      </c>
+      <c r="C55" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>424</v>
+      </c>
+      <c r="B56">
+        <v>539</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more mapping, some constants in code
</commit_message>
<xml_diff>
--- a/Adventure.xlsx
+++ b/Adventure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Adventure-wherigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B75477C-D2E4-4778-B6AF-6F34AC16842C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A77F148-2DA6-4AC6-B1CC-86DBE7B3F0A5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="10790" xr2:uid="{DA9CDC86-6B9C-4A3C-A222-7CC08085C3FF}"/>
   </bookViews>
@@ -2053,8 +2053,8 @@
   <dimension ref="A1:O133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2668,7 +2668,7 @@
         <v>229</v>
       </c>
       <c r="M18" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -3283,12 +3283,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>94</v>
       </c>
       <c r="B34" t="s">
         <v>92</v>
+      </c>
+      <c r="C34">
+        <v>312</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>16</v>
@@ -4293,6 +4296,9 @@
       <c r="B63" t="s">
         <v>172</v>
       </c>
+      <c r="C63">
+        <v>314</v>
+      </c>
       <c r="D63" s="4">
         <v>19</v>
       </c>
@@ -4331,6 +4337,9 @@
       <c r="B64" t="s">
         <v>176</v>
       </c>
+      <c r="C64">
+        <v>152</v>
+      </c>
       <c r="D64" s="4" t="s">
         <v>16</v>
       </c>
@@ -4483,6 +4492,9 @@
       <c r="B68" t="s">
         <v>187</v>
       </c>
+      <c r="C68">
+        <v>153</v>
+      </c>
       <c r="D68" s="4">
         <v>86</v>
       </c>
@@ -6224,6 +6236,12 @@
       <c r="I127" s="4">
         <v>124</v>
       </c>
+      <c r="J127" s="4">
+        <v>5</v>
+      </c>
+      <c r="K127" s="4">
+        <v>122</v>
+      </c>
       <c r="L127" s="4" t="s">
         <v>16</v>
       </c>
@@ -6250,19 +6268,46 @@
       <c r="G128" s="4">
         <v>124</v>
       </c>
-    </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H128" s="4">
+        <v>5</v>
+      </c>
+      <c r="I128" s="4">
+        <v>125</v>
+      </c>
+      <c r="J128" s="4">
+        <v>5</v>
+      </c>
+      <c r="K128" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>349</v>
       </c>
       <c r="C129">
         <v>445</v>
       </c>
+      <c r="D129" s="4">
+        <v>5</v>
+      </c>
+      <c r="E129" s="4">
+        <v>128</v>
+      </c>
+      <c r="F129" s="4">
+        <v>5</v>
+      </c>
       <c r="G129" s="4">
         <v>125</v>
       </c>
-    </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H129" s="4">
+        <v>5</v>
+      </c>
+      <c r="J129" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>543</v>
       </c>
@@ -6273,7 +6318,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>544</v>
       </c>
@@ -6293,7 +6338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>545</v>
       </c>
@@ -6310,7 +6355,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>546</v>
       </c>

</xml_diff>

<commit_message>
more mapping & code cleanup
</commit_message>
<xml_diff>
--- a/Adventure.xlsx
+++ b/Adventure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Adventure-wherigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A77F148-2DA6-4AC6-B1CC-86DBE7B3F0A5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573787B0-C49E-42DB-8E72-2C80220FD38C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="10790" xr2:uid="{DA9CDC86-6B9C-4A3C-A222-7CC08085C3FF}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="559">
   <si>
     <t>Long description</t>
   </si>
@@ -1671,6 +1671,42 @@
   </si>
   <si>
     <t>You  are in an open forest, west of a deep valley.  To the west and south the forest seems to grow denser and gloomier.</t>
+  </si>
+  <si>
+    <t>Dead end</t>
+  </si>
+  <si>
+    <t>You  are  in  a large low circular chamber whose floor is an immense slab fallen from the ceiling (Slab room).  It may be possible to climb one  of the  walls to reach the hole gaping above your head.  East and west there once were large passages, but they are now  filled  with  boulders.   Low small  passages  go north and south, and the south one quickly bends west around the boulders.</t>
+  </si>
+  <si>
+    <t>You're in Slab room.</t>
+  </si>
+  <si>
+    <t>You are at the west end of the Twopit room.  There is a large hole in the wall above the pit at this end of the room.</t>
+  </si>
+  <si>
+    <t>You're at west end of Twopit room.</t>
+  </si>
+  <si>
+    <t>You're in west pit.</t>
+  </si>
+  <si>
+    <t>You  are at the bottom of the western pit in the Twopit room.  There is a large hole in the wall about 25 feet above you.</t>
+  </si>
+  <si>
+    <t>You're at east end of Twopit room.</t>
+  </si>
+  <si>
+    <t>You  are at the bottom of the eastern pit in the Twopit room.  There is a small pool of oil in one corner of the pit.</t>
+  </si>
+  <si>
+    <t>You're in east pit.  There is a small pool of oil here.</t>
+  </si>
+  <si>
+    <t>78 (2/3 of time)</t>
+  </si>
+  <si>
+    <t>75 (2/3 of time)</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1735,6 +1771,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2050,11 +2089,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738AE1BC-ED79-46FF-9BB3-5FA0937E704C}">
-  <dimension ref="A1:O133"/>
+  <dimension ref="A1:O137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86:XFD86"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3334,6 +3373,9 @@
       <c r="B35" t="s">
         <v>93</v>
       </c>
+      <c r="C35">
+        <v>320</v>
+      </c>
       <c r="D35" s="4" t="s">
         <v>16</v>
       </c>
@@ -3365,12 +3407,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>100</v>
       </c>
       <c r="B36" t="s">
         <v>96</v>
+      </c>
+      <c r="C36">
+        <v>319</v>
       </c>
       <c r="D36" s="4">
         <v>37</v>
@@ -3410,6 +3455,9 @@
       <c r="B37" t="s">
         <v>97</v>
       </c>
+      <c r="C37">
+        <v>321</v>
+      </c>
       <c r="D37" s="4">
         <v>36</v>
       </c>
@@ -3448,6 +3496,9 @@
       <c r="B38" t="s">
         <v>102</v>
       </c>
+      <c r="C38">
+        <v>161</v>
+      </c>
       <c r="D38" s="4">
         <v>19</v>
       </c>
@@ -3486,6 +3537,9 @@
       <c r="B39" t="s">
         <v>108</v>
       </c>
+      <c r="C39">
+        <v>395</v>
+      </c>
       <c r="D39" s="4" t="s">
         <v>16</v>
       </c>
@@ -3524,6 +3578,9 @@
       <c r="B40" t="s">
         <v>117</v>
       </c>
+      <c r="C40">
+        <v>394</v>
+      </c>
       <c r="D40" s="4" t="s">
         <v>16</v>
       </c>
@@ -3562,6 +3619,9 @@
       <c r="B41" t="s">
         <v>122</v>
       </c>
+      <c r="C41">
+        <v>162</v>
+      </c>
       <c r="D41" s="4" t="s">
         <v>16</v>
       </c>
@@ -3600,6 +3660,9 @@
       <c r="B42" t="s">
         <v>126</v>
       </c>
+      <c r="C42">
+        <v>196</v>
+      </c>
       <c r="D42" s="4">
         <v>43</v>
       </c>
@@ -3638,6 +3701,9 @@
       <c r="B43" t="s">
         <v>127</v>
       </c>
+      <c r="C43">
+        <v>197</v>
+      </c>
       <c r="D43" s="4" t="s">
         <v>16</v>
       </c>
@@ -3676,6 +3742,9 @@
       <c r="B44" t="s">
         <v>128</v>
       </c>
+      <c r="C44">
+        <v>195</v>
+      </c>
       <c r="D44" s="4">
         <v>42</v>
       </c>
@@ -3711,6 +3780,9 @@
       <c r="B45" t="s">
         <v>132</v>
       </c>
+      <c r="C45">
+        <v>300</v>
+      </c>
       <c r="D45" s="4">
         <v>46</v>
       </c>
@@ -3746,6 +3818,9 @@
       <c r="B46" t="s">
         <v>133</v>
       </c>
+      <c r="C46">
+        <v>310</v>
+      </c>
       <c r="D46" s="4">
         <v>47</v>
       </c>
@@ -3766,12 +3841,18 @@
       </c>
       <c r="J46" s="4">
         <v>51</v>
+      </c>
+      <c r="K46" s="4">
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>134</v>
       </c>
+      <c r="C47">
+        <v>305</v>
+      </c>
       <c r="D47" s="4">
         <v>48</v>
       </c>
@@ -3801,6 +3882,9 @@
       <c r="B48" t="s">
         <v>135</v>
       </c>
+      <c r="C48">
+        <v>302</v>
+      </c>
       <c r="D48" s="4">
         <v>49</v>
       </c>
@@ -3833,6 +3917,9 @@
       <c r="B49" t="s">
         <v>136</v>
       </c>
+      <c r="C49">
+        <v>309</v>
+      </c>
       <c r="D49" s="4">
         <v>50</v>
       </c>
@@ -3853,12 +3940,18 @@
       </c>
       <c r="J49" s="4">
         <v>55</v>
+      </c>
+      <c r="K49" s="4">
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>137</v>
       </c>
+      <c r="C50">
+        <v>306</v>
+      </c>
       <c r="D50" s="4">
         <v>45</v>
       </c>
@@ -3882,6 +3975,9 @@
       <c r="B51" t="s">
         <v>138</v>
       </c>
+      <c r="C51">
+        <v>307</v>
+      </c>
       <c r="D51" s="4">
         <v>52</v>
       </c>
@@ -3911,6 +4007,9 @@
       <c r="B52" t="s">
         <v>139</v>
       </c>
+      <c r="C52">
+        <v>301</v>
+      </c>
       <c r="D52" s="4">
         <v>53</v>
       </c>
@@ -3937,12 +4036,18 @@
       </c>
       <c r="L52" s="4">
         <v>46</v>
+      </c>
+      <c r="M52" s="4">
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>140</v>
       </c>
+      <c r="C53">
+        <v>303</v>
+      </c>
       <c r="D53" s="4">
         <v>54</v>
       </c>
@@ -3969,6 +4074,9 @@
       <c r="B54" t="s">
         <v>141</v>
       </c>
+      <c r="C54">
+        <v>304</v>
+      </c>
       <c r="D54" s="4">
         <v>55</v>
       </c>
@@ -3998,6 +4106,9 @@
       <c r="B55" t="s">
         <v>142</v>
       </c>
+      <c r="C55">
+        <v>308</v>
+      </c>
       <c r="D55" s="4">
         <v>51</v>
       </c>
@@ -4027,8 +4138,14 @@
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>547</v>
+      </c>
       <c r="B56" t="s">
         <v>143</v>
+      </c>
+      <c r="C56">
+        <v>311</v>
       </c>
       <c r="D56" s="4">
         <v>52</v>
@@ -4068,6 +4185,9 @@
       <c r="B57" t="s">
         <v>144</v>
       </c>
+      <c r="C57">
+        <v>313</v>
+      </c>
       <c r="D57" s="4" t="s">
         <v>16</v>
       </c>
@@ -4106,6 +4226,9 @@
       <c r="B58" t="s">
         <v>148</v>
       </c>
+      <c r="C58">
+        <v>316</v>
+      </c>
       <c r="D58" s="4">
         <v>59</v>
       </c>
@@ -4144,6 +4267,9 @@
       <c r="B59" t="s">
         <v>149</v>
       </c>
+      <c r="C59">
+        <v>317</v>
+      </c>
       <c r="D59" s="4">
         <v>60</v>
       </c>
@@ -4182,6 +4308,9 @@
       <c r="B60" t="s">
         <v>151</v>
       </c>
+      <c r="C60">
+        <v>318</v>
+      </c>
       <c r="D60" s="4" t="s">
         <v>16</v>
       </c>
@@ -4220,6 +4349,9 @@
       <c r="B61" t="s">
         <v>155</v>
       </c>
+      <c r="C61">
+        <v>215</v>
+      </c>
       <c r="D61" s="4" t="s">
         <v>16</v>
       </c>
@@ -4258,6 +4390,9 @@
       <c r="B62" t="s">
         <v>157</v>
       </c>
+      <c r="C62">
+        <v>247</v>
+      </c>
       <c r="D62" s="4">
         <v>65</v>
       </c>
@@ -4381,6 +4516,9 @@
       <c r="B65" t="s">
         <v>178</v>
       </c>
+      <c r="C65">
+        <v>210</v>
+      </c>
       <c r="D65" s="4">
         <v>66</v>
       </c>
@@ -4407,6 +4545,9 @@
       </c>
       <c r="L65" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="M65" s="4">
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.35">
@@ -4416,6 +4557,9 @@
       <c r="B66" t="s">
         <v>179</v>
       </c>
+      <c r="C66">
+        <v>237</v>
+      </c>
       <c r="D66" s="4">
         <v>67</v>
       </c>
@@ -4454,6 +4598,9 @@
       <c r="B67" t="s">
         <v>181</v>
       </c>
+      <c r="C67">
+        <v>239</v>
+      </c>
       <c r="D67" s="4" t="s">
         <v>328</v>
       </c>
@@ -4507,6 +4654,24 @@
       <c r="G68" s="4">
         <v>86</v>
       </c>
+      <c r="H68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
@@ -4523,6 +4688,9 @@
       <c r="B70" t="s">
         <v>194</v>
       </c>
+      <c r="C70">
+        <v>207</v>
+      </c>
       <c r="D70" s="4" t="s">
         <v>232</v>
       </c>
@@ -4564,11 +4732,14 @@
       <c r="B71" t="s">
         <v>196</v>
       </c>
+      <c r="C71">
+        <v>208</v>
+      </c>
       <c r="D71" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E71" s="4">
-        <v>75</v>
+      <c r="E71" s="6" t="s">
+        <v>558</v>
       </c>
       <c r="F71" s="4">
         <v>72</v>
@@ -4579,8 +4750,8 @@
       <c r="H71" s="4">
         <v>70</v>
       </c>
-      <c r="I71" s="4">
-        <v>78</v>
+      <c r="I71" s="6" t="s">
+        <v>557</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>16</v>
@@ -4602,6 +4773,9 @@
       <c r="B72" t="s">
         <v>197</v>
       </c>
+      <c r="C72">
+        <v>225</v>
+      </c>
       <c r="D72" s="4" t="s">
         <v>16</v>
       </c>
@@ -4732,11 +4906,44 @@
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>554</v>
+      </c>
       <c r="B77" t="s">
         <v>210</v>
       </c>
+      <c r="C77">
+        <v>157</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F77" s="4">
         <v>71</v>
+      </c>
+      <c r="G77" s="4">
+        <v>135</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L77" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M77" s="4">
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.35">
@@ -4746,6 +4953,9 @@
       <c r="B78" t="s">
         <v>211</v>
       </c>
+      <c r="C78">
+        <v>226</v>
+      </c>
       <c r="D78" s="4">
         <v>79</v>
       </c>
@@ -4816,6 +5026,9 @@
       <c r="B80" t="s">
         <v>217</v>
       </c>
+      <c r="C80">
+        <v>213</v>
+      </c>
       <c r="D80" s="4">
         <v>81</v>
       </c>
@@ -4996,6 +5209,9 @@
       <c r="B86" t="s">
         <v>230</v>
       </c>
+      <c r="C86">
+        <v>167</v>
+      </c>
       <c r="D86" s="4">
         <v>68</v>
       </c>
@@ -5141,6 +5357,9 @@
       <c r="B91" t="s">
         <v>243</v>
       </c>
+      <c r="C91">
+        <v>194</v>
+      </c>
       <c r="D91" s="4">
         <v>42</v>
       </c>
@@ -5577,6 +5796,9 @@
       <c r="B102" t="s">
         <v>281</v>
       </c>
+      <c r="C102">
+        <v>168</v>
+      </c>
       <c r="D102" s="4">
         <v>102</v>
       </c>
@@ -5612,6 +5834,9 @@
       <c r="B103" t="s">
         <v>281</v>
       </c>
+      <c r="C103">
+        <v>171</v>
+      </c>
       <c r="D103" s="4">
         <v>104</v>
       </c>
@@ -5632,6 +5857,9 @@
       <c r="B104" t="s">
         <v>281</v>
       </c>
+      <c r="C104">
+        <v>169</v>
+      </c>
       <c r="D104" s="4">
         <v>104</v>
       </c>
@@ -5646,6 +5874,9 @@
       <c r="B105" t="s">
         <v>285</v>
       </c>
+      <c r="C105">
+        <v>191</v>
+      </c>
       <c r="D105" s="4" t="s">
         <v>16</v>
       </c>
@@ -5684,6 +5915,9 @@
       <c r="B106" t="s">
         <v>281</v>
       </c>
+      <c r="C106">
+        <v>170</v>
+      </c>
       <c r="D106" s="4">
         <v>105</v>
       </c>
@@ -5768,11 +6002,17 @@
       <c r="B109" t="s">
         <v>281</v>
       </c>
+      <c r="C109">
+        <v>173</v>
+      </c>
       <c r="D109" s="4">
         <v>109</v>
       </c>
       <c r="E109" s="4">
         <v>110</v>
+      </c>
+      <c r="L109" s="4">
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.35">
@@ -5782,6 +6022,9 @@
       <c r="B110" t="s">
         <v>281</v>
       </c>
+      <c r="C110">
+        <v>175</v>
+      </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
@@ -6281,7 +6524,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="129" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>349</v>
       </c>
@@ -6307,7 +6550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>543</v>
       </c>
@@ -6318,7 +6561,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="131" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>544</v>
       </c>
@@ -6338,7 +6581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>545</v>
       </c>
@@ -6355,7 +6598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>546</v>
       </c>
@@ -6367,6 +6610,170 @@
       </c>
       <c r="F133" s="4">
         <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>549</v>
+      </c>
+      <c r="B134" t="s">
+        <v>548</v>
+      </c>
+      <c r="C134">
+        <v>209</v>
+      </c>
+      <c r="D134" s="4">
+        <v>70</v>
+      </c>
+      <c r="E134" s="4">
+        <v>135</v>
+      </c>
+      <c r="F134" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G134" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H134" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J134" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K134" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L134" s="4">
+        <v>65</v>
+      </c>
+      <c r="M134" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>551</v>
+      </c>
+      <c r="B135" t="s">
+        <v>550</v>
+      </c>
+      <c r="C135">
+        <v>156</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F135" s="4">
+        <v>77</v>
+      </c>
+      <c r="G135" s="4">
+        <v>134</v>
+      </c>
+      <c r="H135" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J135" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K135" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L135" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M135" s="4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>552</v>
+      </c>
+      <c r="B136" t="s">
+        <v>553</v>
+      </c>
+      <c r="C136">
+        <v>159</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K136" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L136" s="4">
+        <v>135</v>
+      </c>
+      <c r="M136" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>556</v>
+      </c>
+      <c r="B137" t="s">
+        <v>555</v>
+      </c>
+      <c r="C137">
+        <v>158</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L137" s="4">
+        <v>77</v>
+      </c>
+      <c r="M137" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -6855,7 +7262,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D17"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Start of actual cartridge
</commit_message>
<xml_diff>
--- a/Adventure.xlsx
+++ b/Adventure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Adventure-wherigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418A8188-FA8E-41C6-AE64-996FF43B7290}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999B2F3E-5FFC-4786-BF98-F8B244728C68}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="9850" xr2:uid="{DA9CDC86-6B9C-4A3C-A222-7CC08085C3FF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="verbs" sheetId="5" r:id="rId5"/>
     <sheet name="nouns" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2269" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2270" uniqueCount="731">
   <si>
     <t>Long description</t>
   </si>
@@ -2220,6 +2220,9 @@
   </si>
   <si>
     <t>You're in small, icy chamber.</t>
+  </si>
+  <si>
+    <t>thurb -&gt; 221</t>
   </si>
 </sst>
 </file>
@@ -2605,8 +2608,8 @@
   <dimension ref="A1:P258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H263" sqref="H263"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12577,7 +12580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>719</v>
       </c>
@@ -12621,7 +12624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>729</v>
       </c>
@@ -12663,6 +12666,9 @@
       </c>
       <c r="N258" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="O258" s="4" t="s">
+        <v>730</v>
       </c>
     </row>
   </sheetData>

</xml_diff>